<commit_message>
fixed na and new data
</commit_message>
<xml_diff>
--- a/data/bsc201_community_lab_data.xlsx
+++ b/data/bsc201_community_lab_data.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wlperry/Desktop/bsc201_comm_ecol/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wlperry/Documents/r_projects/bsc201_comm_ecol/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C0E7C4D-0F13-FF41-B1EC-3992ED87AD4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D33A488-60A2-C04B-BCC5-8C9C049DB21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49620" yWindow="4740" windowWidth="27700" windowHeight="16940" xr2:uid="{27A33AFF-BB58-E540-A561-21EAB5E80E3D}"/>
+    <workbookView xWindow="1000" yWindow="780" windowWidth="19180" windowHeight="10060" xr2:uid="{27A33AFF-BB58-E540-A561-21EAB5E80E3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,27 +38,42 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
+    <t>restoration_status</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>aquatic_shannon_diversity</t>
+  </si>
+  <si>
+    <t>terrestrial_shannon_diversity</t>
+  </si>
+  <si>
+    <t>plant_richness</t>
+  </si>
+  <si>
     <t>Restored Sites</t>
   </si>
   <si>
+    <t>Fairview Park</t>
+  </si>
+  <si>
+    <t>Anderson Park</t>
+  </si>
+  <si>
+    <t>Epiphany Church</t>
+  </si>
+  <si>
+    <t>College Hills</t>
+  </si>
+  <si>
+    <t>Hidden Creek</t>
+  </si>
+  <si>
     <t>Unrestored Sites</t>
   </si>
   <si>
-    <t>Fairview Park</t>
-  </si>
-  <si>
-    <t>Anderson Park</t>
-  </si>
-  <si>
-    <t>Epiphany Church</t>
-  </si>
-  <si>
-    <t>College Hills</t>
-  </si>
-  <si>
-    <t>Hidden Creek</t>
-  </si>
-  <si>
     <t>Oakdale</t>
   </si>
   <si>
@@ -72,21 +87,6 @@
   </si>
   <si>
     <t>Blaire</t>
-  </si>
-  <si>
-    <t>aquatic_shannon_diversity</t>
-  </si>
-  <si>
-    <t>terrestrial_shannon_diversity</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>restoration_status</t>
-  </si>
-  <si>
-    <t>plant_richness</t>
   </si>
 </sst>
 </file>
@@ -460,204 +460,197 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>0.27700000000000002</v>
       </c>
       <c r="D2">
-        <v>4.0999999999999996</v>
+        <v>1.835</v>
       </c>
       <c r="E2">
-        <v>1.2</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>3.4</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>4.2</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="E3">
-        <v>1.3</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>2.4</v>
+        <v>1.579</v>
       </c>
       <c r="D4">
-        <v>4.3</v>
+        <v>0.77300000000000002</v>
       </c>
       <c r="E4">
-        <v>1.4</v>
+        <v>3.78</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>3.1</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="D5">
-        <v>3.2</v>
+        <v>0.96499999999999997</v>
       </c>
       <c r="E5">
-        <v>1.1000000000000001</v>
+        <v>3.56</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>2.9</v>
+        <v>0.69599999999999995</v>
       </c>
       <c r="D6">
-        <v>3.9</v>
+        <v>0.502</v>
       </c>
       <c r="E6">
-        <v>1.5</v>
+        <v>2.4700000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>1.3</v>
+        <v>1.127</v>
       </c>
       <c r="D7">
-        <v>2.1</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="E7">
-        <v>0.6</v>
+        <v>4.83</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>1.4</v>
+        <v>13</v>
       </c>
       <c r="D8">
-        <v>2.2000000000000002</v>
+        <v>0.86899999999999999</v>
       </c>
       <c r="E8">
-        <v>0.5</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>1.2</v>
+        <v>0.874</v>
       </c>
       <c r="D9">
-        <v>3.1</v>
+        <v>1.252</v>
       </c>
       <c r="E9">
-        <v>0.7</v>
+        <v>4.3899999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C10">
-        <v>1.2</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="D10">
-        <v>3.2</v>
+        <v>1.7270000000000001</v>
       </c>
       <c r="E10">
-        <v>0.4</v>
+        <v>2.73</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <v>1.1000000000000001</v>
+        <v>1.4279999999999999</v>
       </c>
       <c r="D11">
-        <v>3.1</v>
+        <v>0.97399999999999998</v>
       </c>
       <c r="E11">
-        <v>0.8</v>
+        <v>2.72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>